<commit_message>
Updated csv/xlsx sheet + js file
- Added image URLs in csv/xlsx
- Added yesterday's tapioca
- JSON data for JS
</commit_message>
<xml_diff>
--- a/tapiocount_sheet.xlsx
+++ b/tapiocount_sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="tapiocount_sheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="284">
   <si>
     <t>Date</t>
   </si>
@@ -53,9 +53,6 @@
     <t>SF</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>85 Degrees</t>
   </si>
   <si>
@@ -335,9 +332,6 @@
     <t>SF (FiDi)</t>
   </si>
   <si>
-    <t>Cassava Café</t>
-  </si>
-  <si>
     <t>TJ Cups</t>
   </si>
   <si>
@@ -470,9 +464,6 @@
     <t>Roasted oolong milk tea</t>
   </si>
   <si>
-    <t>Sweetheart Café</t>
-  </si>
-  <si>
     <t>Steap</t>
   </si>
   <si>
@@ -879,6 +870,12 @@
   </si>
   <si>
     <t>https://farm5.staticflickr.com/4595/27436513069_4d74fb90d6_z.jpg</t>
+  </si>
+  <si>
+    <t>Cassava Cafe</t>
+  </si>
+  <si>
+    <t>Sweetheart Cafe</t>
   </si>
 </sst>
 </file>
@@ -886,7 +883,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -926,10 +923,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1239,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1258,25 +1255,19 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42756</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1284,16 +1275,13 @@
         <v>42756</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1301,16 +1289,13 @@
         <v>42762</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1318,19 +1303,19 @@
         <v>42769</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>282</v>
       </c>
       <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1338,13 +1323,13 @@
         <v>42770</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1352,16 +1337,13 @@
         <v>42770</v>
       </c>
       <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1369,13 +1351,13 @@
         <v>42774</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1383,16 +1365,16 @@
         <v>42779</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1400,16 +1382,16 @@
         <v>42784</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1419,16 +1401,16 @@
         <v>42791</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1436,19 +1418,19 @@
         <v>42798</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1456,16 +1438,16 @@
         <v>42804</v>
       </c>
       <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
       <c r="E14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1473,16 +1455,16 @@
         <v>42805</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1490,16 +1472,16 @@
         <v>42806</v>
       </c>
       <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1507,16 +1489,16 @@
         <v>42812</v>
       </c>
       <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
       <c r="E17" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1524,19 +1506,19 @@
         <v>42813</v>
       </c>
       <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>40</v>
       </c>
-      <c r="D18" t="s">
-        <v>41</v>
-      </c>
       <c r="E18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F18" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1544,19 +1526,19 @@
         <v>42817</v>
       </c>
       <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" t="s">
-        <v>43</v>
-      </c>
       <c r="E19" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F19" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1564,16 +1546,16 @@
         <v>42829</v>
       </c>
       <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1581,13 +1563,13 @@
         <v>42832</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1595,19 +1577,19 @@
         <v>42834</v>
       </c>
       <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
         <v>47</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>48</v>
       </c>
-      <c r="D22" t="s">
-        <v>49</v>
-      </c>
       <c r="E22" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F22" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1615,19 +1597,19 @@
         <v>42835</v>
       </c>
       <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
         <v>25</v>
       </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" t="s">
-        <v>26</v>
-      </c>
       <c r="E23" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F23" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1635,16 +1617,16 @@
         <v>42836</v>
       </c>
       <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
         <v>51</v>
       </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1652,16 +1634,16 @@
         <v>42846</v>
       </c>
       <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
         <v>53</v>
       </c>
-      <c r="C25" t="s">
-        <v>54</v>
-      </c>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E25" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1669,16 +1651,16 @@
         <v>42848</v>
       </c>
       <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
         <v>55</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>56</v>
       </c>
-      <c r="D26" t="s">
-        <v>57</v>
-      </c>
       <c r="E26" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1686,19 +1668,19 @@
         <v>42854</v>
       </c>
       <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
         <v>58</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>59</v>
       </c>
-      <c r="D27" t="s">
-        <v>60</v>
-      </c>
       <c r="E27" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F27" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1706,7 +1688,7 @@
         <v>42855</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -1715,7 +1697,7 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1723,19 +1705,19 @@
         <v>42870</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F29" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1743,16 +1725,16 @@
         <v>42877</v>
       </c>
       <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
       <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1760,16 +1742,16 @@
         <v>42880</v>
       </c>
       <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
         <v>64</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>65</v>
       </c>
-      <c r="D31" t="s">
-        <v>66</v>
-      </c>
       <c r="E31" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1777,16 +1759,16 @@
         <v>42881</v>
       </c>
       <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
         <v>67</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>68</v>
       </c>
-      <c r="D32" t="s">
-        <v>69</v>
-      </c>
       <c r="E32" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1794,16 +1776,16 @@
         <v>42890</v>
       </c>
       <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
         <v>70</v>
       </c>
-      <c r="C33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" t="s">
-        <v>71</v>
-      </c>
       <c r="E33" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1811,16 +1793,16 @@
         <v>42891</v>
       </c>
       <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
         <v>22</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>23</v>
       </c>
-      <c r="D34" t="s">
-        <v>24</v>
-      </c>
       <c r="E34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1831,13 +1813,13 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1845,16 +1827,16 @@
         <v>42897</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1862,16 +1844,16 @@
         <v>42899</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1879,19 +1861,19 @@
         <v>42901</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F38" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1899,16 +1881,16 @@
         <v>42902</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1916,16 +1898,16 @@
         <v>42904</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1933,16 +1915,16 @@
         <v>42914</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D41" t="s">
         <v>8</v>
       </c>
       <c r="E41" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1950,19 +1932,19 @@
         <v>42918</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F42" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1970,16 +1952,16 @@
         <v>42919</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1987,19 +1969,19 @@
         <v>42920</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E44" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F44" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2007,13 +1989,13 @@
         <v>42924</v>
       </c>
       <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
         <v>47</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>48</v>
-      </c>
-      <c r="D45" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2021,19 +2003,19 @@
         <v>42926</v>
       </c>
       <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>23</v>
       </c>
-      <c r="D46" t="s">
-        <v>24</v>
-      </c>
       <c r="E46" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F46" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2041,16 +2023,16 @@
         <v>42927</v>
       </c>
       <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
         <v>80</v>
       </c>
-      <c r="C47" t="s">
-        <v>81</v>
-      </c>
       <c r="D47" t="s">
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2058,19 +2040,19 @@
         <v>42929</v>
       </c>
       <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
         <v>82</v>
       </c>
-      <c r="C48" t="s">
-        <v>83</v>
-      </c>
       <c r="D48" t="s">
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F48" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2078,19 +2060,19 @@
         <v>42930</v>
       </c>
       <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
         <v>84</v>
       </c>
-      <c r="C49" t="s">
-        <v>85</v>
-      </c>
       <c r="D49" t="s">
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F49" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2098,19 +2080,19 @@
         <v>42932</v>
       </c>
       <c r="B50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" t="s">
         <v>86</v>
       </c>
-      <c r="C50" t="s">
-        <v>125</v>
-      </c>
-      <c r="D50" t="s">
-        <v>87</v>
-      </c>
       <c r="E50" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F50" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2118,16 +2100,16 @@
         <v>42934</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D51" t="s">
         <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2135,16 +2117,16 @@
         <v>42936</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" t="s">
         <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2152,19 +2134,19 @@
         <v>42940</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D53" t="s">
         <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F53" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2172,16 +2154,16 @@
         <v>42945</v>
       </c>
       <c r="B54" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" t="s">
         <v>88</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>89</v>
       </c>
-      <c r="D54" t="s">
-        <v>90</v>
-      </c>
       <c r="E54" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2189,16 +2171,16 @@
         <v>42951</v>
       </c>
       <c r="B55" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" t="s">
         <v>91</v>
       </c>
-      <c r="C55" t="s">
-        <v>127</v>
-      </c>
-      <c r="D55" t="s">
-        <v>92</v>
-      </c>
       <c r="E55" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2206,16 +2188,16 @@
         <v>42951</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E56" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2223,16 +2205,16 @@
         <v>42953</v>
       </c>
       <c r="B57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" t="s">
         <v>95</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>96</v>
       </c>
-      <c r="D57" t="s">
-        <v>97</v>
-      </c>
       <c r="E57" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2240,16 +2222,16 @@
         <v>42954</v>
       </c>
       <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" t="s">
         <v>98</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>99</v>
       </c>
-      <c r="D58" t="s">
-        <v>100</v>
-      </c>
       <c r="E58" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2257,19 +2239,19 @@
         <v>42957</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F59" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2277,16 +2259,16 @@
         <v>42960</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
         <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2294,19 +2276,19 @@
         <v>42962</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E61" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F61" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2314,7 +2296,7 @@
         <v>42963</v>
       </c>
       <c r="B62" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
@@ -2323,7 +2305,7 @@
         <v>8</v>
       </c>
       <c r="E62" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2331,19 +2313,19 @@
         <v>42972</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D63" t="s">
         <v>8</v>
       </c>
       <c r="E63" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F63" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2351,16 +2333,16 @@
         <v>42973</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2368,10 +2350,10 @@
         <v>42983</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D65" t="s">
         <v>8</v>
@@ -2382,13 +2364,13 @@
         <v>42984</v>
       </c>
       <c r="B66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2396,7 +2378,7 @@
         <v>42985</v>
       </c>
       <c r="B67" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C67" t="s">
         <v>7</v>
@@ -2410,16 +2392,16 @@
         <v>42988</v>
       </c>
       <c r="B68" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C68" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D68" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E68" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2427,13 +2409,13 @@
         <v>42989</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D69" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2441,16 +2423,16 @@
         <v>42993</v>
       </c>
       <c r="B70" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C70" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D70" t="s">
         <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2458,19 +2440,19 @@
         <v>42994</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D71" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E71" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F71" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2478,19 +2460,19 @@
         <v>42995</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D72" t="s">
         <v>8</v>
       </c>
       <c r="E72" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F72" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2498,16 +2480,16 @@
         <v>42996</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C73" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D73" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E73" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2515,16 +2497,16 @@
         <v>42999</v>
       </c>
       <c r="B74" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C74" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D74" t="s">
         <v>8</v>
       </c>
       <c r="E74" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2532,16 +2514,16 @@
         <v>43000</v>
       </c>
       <c r="B75" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C75" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D75" t="s">
         <v>8</v>
       </c>
       <c r="E75" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2549,19 +2531,19 @@
         <v>43001</v>
       </c>
       <c r="B76" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C76" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
       </c>
       <c r="E76" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F76" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2569,16 +2551,16 @@
         <v>43002</v>
       </c>
       <c r="B77" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C77" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E77" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2586,19 +2568,19 @@
         <v>43006</v>
       </c>
       <c r="B78" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D78" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E78" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F78" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2606,16 +2588,16 @@
         <v>43009</v>
       </c>
       <c r="B79" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C79" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D79" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E79" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2623,16 +2605,16 @@
         <v>43016</v>
       </c>
       <c r="B80" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C80" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D80" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E80" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2640,16 +2622,16 @@
         <v>43017</v>
       </c>
       <c r="B81" t="s">
+        <v>140</v>
+      </c>
+      <c r="C81" t="s">
         <v>142</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>144</v>
       </c>
-      <c r="D81" t="s">
-        <v>146</v>
-      </c>
       <c r="E81" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2657,16 +2639,16 @@
         <v>43018</v>
       </c>
       <c r="B82" t="s">
+        <v>141</v>
+      </c>
+      <c r="C82" t="s">
         <v>143</v>
       </c>
-      <c r="C82" t="s">
-        <v>145</v>
-      </c>
       <c r="D82" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E82" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2674,16 +2656,16 @@
         <v>43021</v>
       </c>
       <c r="B83" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C83" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D83" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E83" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2691,16 +2673,16 @@
         <v>43023</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C84" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D84" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E84" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2708,16 +2690,16 @@
         <v>43024</v>
       </c>
       <c r="B85" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D85" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E85" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2725,19 +2707,19 @@
         <v>43030</v>
       </c>
       <c r="B86" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C86" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D86" t="s">
         <v>8</v>
       </c>
       <c r="E86" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F86" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2745,19 +2727,19 @@
         <v>43031</v>
       </c>
       <c r="B87" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C87" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D87" t="s">
         <v>8</v>
       </c>
       <c r="E87" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F87" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -2765,16 +2747,16 @@
         <v>43036</v>
       </c>
       <c r="B88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C88" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D88" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E88" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -2782,19 +2764,19 @@
         <v>43037</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C89" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D89" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E89" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F89" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2802,16 +2784,16 @@
         <v>43041</v>
       </c>
       <c r="B90" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C90" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D90" t="s">
         <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -2819,16 +2801,16 @@
         <v>43043</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -2836,16 +2818,16 @@
         <v>43049</v>
       </c>
       <c r="B92" t="s">
-        <v>148</v>
+        <v>283</v>
       </c>
       <c r="C92" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D92" t="s">
         <v>8</v>
       </c>
       <c r="E92" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -2853,16 +2835,16 @@
         <v>43057</v>
       </c>
       <c r="B93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C93" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D93" t="s">
         <v>8</v>
       </c>
       <c r="E93" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2870,19 +2852,19 @@
         <v>43059</v>
       </c>
       <c r="B94" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C94" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D94" t="s">
         <v>8</v>
       </c>
       <c r="E94" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F94" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -2890,16 +2872,16 @@
         <v>43060</v>
       </c>
       <c r="B95" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C95" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D95" t="s">
         <v>8</v>
       </c>
       <c r="E95" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -2907,16 +2889,16 @@
         <v>43062</v>
       </c>
       <c r="B96" t="s">
+        <v>61</v>
+      </c>
+      <c r="C96" t="s">
         <v>62</v>
       </c>
-      <c r="C96" t="s">
-        <v>63</v>
-      </c>
       <c r="D96" t="s">
         <v>8</v>
       </c>
       <c r="E96" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -2924,19 +2906,19 @@
         <v>43063</v>
       </c>
       <c r="B97" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97" t="s">
+        <v>153</v>
+      </c>
+      <c r="D97" t="s">
         <v>25</v>
       </c>
-      <c r="C97" t="s">
-        <v>156</v>
-      </c>
-      <c r="D97" t="s">
-        <v>26</v>
-      </c>
       <c r="E97" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F97" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -2944,16 +2926,16 @@
         <v>43064</v>
       </c>
       <c r="B98" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C98" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D98" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E98" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -2961,19 +2943,19 @@
         <v>43071</v>
       </c>
       <c r="B99" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C99" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D99" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E99" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -2981,19 +2963,19 @@
         <v>43072</v>
       </c>
       <c r="B100" t="s">
+        <v>109</v>
+      </c>
+      <c r="C100" t="s">
+        <v>110</v>
+      </c>
+      <c r="D100" t="s">
         <v>111</v>
       </c>
-      <c r="C100" t="s">
-        <v>112</v>
-      </c>
-      <c r="D100" t="s">
-        <v>113</v>
-      </c>
       <c r="E100" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F100" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -3001,16 +2983,13 @@
         <v>43075</v>
       </c>
       <c r="B101" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C101" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D101" t="s">
         <v>8</v>
-      </c>
-      <c r="E101" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -3018,19 +2997,19 @@
         <v>43084</v>
       </c>
       <c r="B102" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C102" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D102" t="s">
         <v>8</v>
       </c>
       <c r="E102" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F102" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -3038,19 +3017,19 @@
         <v>43085</v>
       </c>
       <c r="B103" t="s">
+        <v>105</v>
+      </c>
+      <c r="C103" t="s">
+        <v>106</v>
+      </c>
+      <c r="D103" t="s">
         <v>107</v>
       </c>
-      <c r="C103" t="s">
-        <v>108</v>
-      </c>
-      <c r="D103" t="s">
-        <v>109</v>
-      </c>
       <c r="E103" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F103" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -3058,16 +3037,16 @@
         <v>43088</v>
       </c>
       <c r="B104" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C104" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D104" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E104" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>